<commit_message>
SMF036. Agregar nuevos campos en plantilla Excel para clientes
</commit_message>
<xml_diff>
--- a/project_files/files/templates/clientes.xlsx
+++ b/project_files/files/templates/clientes.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\simma-facturacion\project_files\files\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="761"/>
   </bookViews>
@@ -28,7 +33,7 @@
     <author>RRamirez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AD1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AI1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AJ1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -316,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AK1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AM1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +379,7 @@
     <author>RRamirez</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -398,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -446,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -518,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -542,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -590,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -614,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -638,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -662,7 +667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -686,7 +691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AH1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -710,7 +715,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AI1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -734,7 +739,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AM1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -758,7 +763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AN1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -787,7 +792,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
   <si>
     <t>No.</t>
   </si>
@@ -973,6 +978,57 @@
   </si>
   <si>
     <t>Nombre Corto</t>
+  </si>
+  <si>
+    <t>Categoria del cliente</t>
+  </si>
+  <si>
+    <t>Moneda</t>
+  </si>
+  <si>
+    <t>Uso del CFDI</t>
+  </si>
+  <si>
+    <t>Clave del Producto o Servicio</t>
+  </si>
+  <si>
+    <t>Clave de Unidad</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Impuesto</t>
+  </si>
+  <si>
+    <t>Tipo de Factor</t>
+  </si>
+  <si>
+    <t>Tasa O Cuota</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>CLABE</t>
+  </si>
+  <si>
+    <t>RFC del Banco</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>Forma de Pago</t>
+  </si>
+  <si>
+    <t>Método de Pago CFDI</t>
   </si>
 </sst>
 </file>
@@ -1048,9 +1104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1351,7 +1408,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1359,13 +1416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE1"/>
+  <dimension ref="A1:BV1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC1" sqref="BC1"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="BT2" sqref="BT2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1424,9 +1481,21 @@
     <col min="55" max="55" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="22" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="19" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="27.7109375" customWidth="1"/>
+    <col min="59" max="60" width="19.85546875" customWidth="1"/>
+    <col min="61" max="61" width="28.85546875" customWidth="1"/>
+    <col min="62" max="62" width="17.42578125" customWidth="1"/>
+    <col min="63" max="63" width="38.28515625" customWidth="1"/>
+    <col min="64" max="64" width="21.85546875" customWidth="1"/>
+    <col min="66" max="66" width="13.42578125" customWidth="1"/>
+    <col min="67" max="67" width="19" customWidth="1"/>
+    <col min="68" max="68" width="18.42578125" customWidth="1"/>
+    <col min="69" max="69" width="17.28515625" customWidth="1"/>
+    <col min="71" max="71" width="19.28515625" customWidth="1"/>
+    <col min="72" max="72" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1597,6 +1666,57 @@
       </c>
       <c r="BE1" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +1732,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
SMF036Y38. Agregar campos en plantillas de Excel y poder importarlos
</commit_message>
<xml_diff>
--- a/project_files/files/templates/clientes.xlsx
+++ b/project_files/files/templates/clientes.xlsx
@@ -16,7 +16,7 @@
     <sheet name="GENERADORES" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GENERADORES!$A$1:$BC$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GENERADORES!$A$1:$BD$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -31,6 +31,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>RRamirez</author>
+    <author>FROSTBITEinternex</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
@@ -273,7 +274,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0">
+    <comment ref="AI1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0">
+    <comment ref="AK1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -321,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0">
+    <comment ref="AL1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0">
+    <comment ref="AN1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -366,6 +392,266 @@
           </rPr>
           <t xml:space="preserve">
 El valor debe corresponder con el catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BG1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">CarlosGutiérrez:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BH1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BI1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BJ1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BK1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BL1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BM1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BO1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BP1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BQ1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
         </r>
       </text>
     </comment>
@@ -377,6 +663,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>RRamirez</author>
+    <author>FROSTBITEinternex</author>
   </authors>
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0">
@@ -739,7 +1026,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>CarlosGutiérrez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El valor debe corresponder con el
+catalogo del sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -763,7 +1075,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0">
+    <comment ref="AO1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -792,7 +1104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>No.</t>
   </si>
@@ -1029,13 +1341,16 @@
   </si>
   <si>
     <t>Método de Pago CFDI</t>
+  </si>
+  <si>
+    <t>Unidad de Facturación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,6 +1388,32 @@
     <font>
       <b/>
       <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -1416,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV1"/>
+  <dimension ref="A1:BW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="BT2" sqref="BT2"/>
+    <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="BT11" sqref="BT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,44 +1799,45 @@
     <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="22" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="27.7109375" customWidth="1"/>
-    <col min="59" max="60" width="19.85546875" customWidth="1"/>
-    <col min="61" max="61" width="28.85546875" customWidth="1"/>
-    <col min="62" max="62" width="17.42578125" customWidth="1"/>
-    <col min="63" max="63" width="38.28515625" customWidth="1"/>
-    <col min="64" max="64" width="21.85546875" customWidth="1"/>
-    <col min="66" max="66" width="13.42578125" customWidth="1"/>
-    <col min="67" max="67" width="19" customWidth="1"/>
-    <col min="68" max="68" width="18.42578125" customWidth="1"/>
-    <col min="69" max="69" width="17.28515625" customWidth="1"/>
-    <col min="71" max="71" width="19.28515625" customWidth="1"/>
-    <col min="72" max="72" width="18.7109375" customWidth="1"/>
+    <col min="35" max="35" width="29.85546875" customWidth="1"/>
+    <col min="36" max="36" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="27.7109375" customWidth="1"/>
+    <col min="60" max="61" width="19.85546875" customWidth="1"/>
+    <col min="62" max="62" width="28.85546875" customWidth="1"/>
+    <col min="63" max="63" width="17.42578125" customWidth="1"/>
+    <col min="64" max="64" width="38.28515625" customWidth="1"/>
+    <col min="65" max="65" width="21.85546875" customWidth="1"/>
+    <col min="67" max="67" width="13.42578125" customWidth="1"/>
+    <col min="68" max="68" width="19" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" customWidth="1"/>
+    <col min="70" max="70" width="17.28515625" customWidth="1"/>
+    <col min="72" max="72" width="19.28515625" customWidth="1"/>
+    <col min="73" max="73" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1599,123 +1941,126 @@
         <v>27</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1728,9 +2073,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1772,27 +2119,28 @@
     <col min="36" max="36" width="9" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29.140625" customWidth="1"/>
+    <col min="40" max="40" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1908,57 +2256,60 @@
         <v>27</v>
       </c>
       <c r="AM1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>